<commit_message>
delrt tree md bom
</commit_message>
<xml_diff>
--- a/datasheet/bom.xlsx
+++ b/datasheet/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="203">
   <si>
     <t xml:space="preserve">Bill of material</t>
   </si>
@@ -457,7 +457,7 @@
     <t xml:space="preserve">pewter_foot2.FCStd</t>
   </si>
   <si>
-    <t xml:space="preserve">tip metal pyramid</t>
+    <t xml:space="preserve">bearing pad</t>
   </si>
   <si>
     <t xml:space="preserve">sub assembly</t>
@@ -617,6 +617,18 @@
   </si>
   <si>
     <t xml:space="preserve">right </t>
+  </si>
+  <si>
+    <t xml:space="preserve">closable back cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lockable back cover with guide rods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">back_cover_stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connects the final whole assembly</t>
   </si>
 </sst>
 </file>
@@ -631,6 +643,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -651,32 +664,38 @@
       <sz val="36"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -727,7 +746,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,6 +763,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -757,14 +780,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -795,9 +810,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>572040</xdr:colOff>
+      <xdr:colOff>571680</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -810,8 +825,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7382880" y="2097360"/>
-          <a:ext cx="504360" cy="323280"/>
+          <a:off x="7394400" y="2097360"/>
+          <a:ext cx="504000" cy="322920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -832,9 +847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>592560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>57960</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -847,8 +862,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8245080" y="2577960"/>
-          <a:ext cx="475560" cy="275760"/>
+          <a:off x="8257680" y="2577960"/>
+          <a:ext cx="475200" cy="275400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -869,9 +884,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>683280</xdr:colOff>
+      <xdr:colOff>682920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -884,8 +899,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7475040" y="2669040"/>
-          <a:ext cx="523440" cy="399600"/>
+          <a:off x="7486560" y="2669040"/>
+          <a:ext cx="523080" cy="399240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -906,9 +921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>529920</xdr:colOff>
+      <xdr:colOff>529560</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,8 +936,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8134560" y="3012480"/>
-          <a:ext cx="523440" cy="323280"/>
+          <a:off x="8147160" y="3012480"/>
+          <a:ext cx="523080" cy="322920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -943,9 +958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>628560</xdr:colOff>
+      <xdr:colOff>628200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -958,8 +973,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7420320" y="3348360"/>
-          <a:ext cx="523440" cy="332640"/>
+          <a:off x="7431840" y="3348360"/>
+          <a:ext cx="523080" cy="332280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,9 +995,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>639360</xdr:colOff>
+      <xdr:colOff>639000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -995,8 +1010,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7431120" y="3795480"/>
-          <a:ext cx="523440" cy="447120"/>
+          <a:off x="7442640" y="3795480"/>
+          <a:ext cx="523080" cy="446760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1017,9 +1032,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>461160</xdr:colOff>
+      <xdr:colOff>460800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1032,8 +1047,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8399160" y="4614120"/>
-          <a:ext cx="190080" cy="704160"/>
+          <a:off x="8411760" y="4614120"/>
+          <a:ext cx="189720" cy="703800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1054,9 +1069,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>299160</xdr:colOff>
+      <xdr:colOff>298800</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1069,8 +1084,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8189640" y="5251680"/>
-          <a:ext cx="237600" cy="437400"/>
+          <a:off x="8202240" y="5251680"/>
+          <a:ext cx="237240" cy="437040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1091,9 +1106,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>652680</xdr:colOff>
+      <xdr:colOff>652320</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1106,8 +1121,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7444440" y="5636880"/>
-          <a:ext cx="523440" cy="304200"/>
+          <a:off x="7455960" y="5636880"/>
+          <a:ext cx="523080" cy="303840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1128,9 +1143,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>542160</xdr:colOff>
+      <xdr:colOff>541800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1143,8 +1158,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8146800" y="5968080"/>
-          <a:ext cx="523440" cy="275760"/>
+          <a:off x="8159400" y="5968080"/>
+          <a:ext cx="523080" cy="275400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1165,9 +1180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>540360</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1180,8 +1195,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8145360" y="6471000"/>
-          <a:ext cx="523440" cy="399600"/>
+          <a:off x="8157960" y="6471000"/>
+          <a:ext cx="523080" cy="399240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1202,9 +1217,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>603360</xdr:colOff>
+      <xdr:colOff>603000</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,8 +1232,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7395120" y="6739560"/>
-          <a:ext cx="523440" cy="408960"/>
+          <a:off x="7406640" y="6739560"/>
+          <a:ext cx="523080" cy="408600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1239,9 +1254,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>529920</xdr:colOff>
+      <xdr:colOff>529560</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1254,8 +1269,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8269920" y="7016400"/>
-          <a:ext cx="388080" cy="416160"/>
+          <a:off x="8282520" y="7016400"/>
+          <a:ext cx="387720" cy="415800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,9 +1291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>597240</xdr:colOff>
+      <xdr:colOff>596880</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1291,8 +1306,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7389000" y="7372080"/>
-          <a:ext cx="523440" cy="332640"/>
+          <a:off x="7400520" y="7372080"/>
+          <a:ext cx="523080" cy="332280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1313,9 +1328,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>622080</xdr:colOff>
+      <xdr:colOff>621720</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1328,8 +1343,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8226720" y="7733520"/>
-          <a:ext cx="523440" cy="361440"/>
+          <a:off x="8239320" y="7733520"/>
+          <a:ext cx="523080" cy="361080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1350,9 +1365,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>597600</xdr:colOff>
+      <xdr:colOff>597240</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1365,8 +1380,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7389360" y="8058600"/>
-          <a:ext cx="523440" cy="351720"/>
+          <a:off x="7400880" y="8058600"/>
+          <a:ext cx="523080" cy="351360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1387,9 +1402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>566280</xdr:colOff>
+      <xdr:colOff>565920</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1402,8 +1417,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8220240" y="8341200"/>
-          <a:ext cx="474120" cy="379080"/>
+          <a:off x="8232840" y="8341200"/>
+          <a:ext cx="473760" cy="378720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1424,9 +1439,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>572760</xdr:colOff>
+      <xdr:colOff>572400</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1439,8 +1454,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7364520" y="8720280"/>
-          <a:ext cx="523440" cy="380520"/>
+          <a:off x="7376040" y="8720280"/>
+          <a:ext cx="523080" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1461,9 +1476,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>566640</xdr:colOff>
+      <xdr:colOff>566280</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>145080</xdr:rowOff>
+      <xdr:rowOff>144720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1476,8 +1491,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8171280" y="9015480"/>
-          <a:ext cx="523440" cy="428040"/>
+          <a:off x="8183880" y="9015480"/>
+          <a:ext cx="523080" cy="427680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1498,9 +1513,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>591120</xdr:colOff>
+      <xdr:colOff>590760</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>115200</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1513,8 +1528,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7382880" y="9358200"/>
-          <a:ext cx="523440" cy="380520"/>
+          <a:off x="7394400" y="9358200"/>
+          <a:ext cx="523080" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1535,9 +1550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>615960</xdr:colOff>
+      <xdr:colOff>615600</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1550,8 +1565,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8220600" y="9749520"/>
-          <a:ext cx="523440" cy="285120"/>
+          <a:off x="8233200" y="9749520"/>
+          <a:ext cx="523080" cy="284760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1572,9 +1587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541440</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1587,8 +1602,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7333560" y="10062720"/>
-          <a:ext cx="523440" cy="218520"/>
+          <a:off x="7345080" y="10062720"/>
+          <a:ext cx="523080" cy="218160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1609,9 +1624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>560160</xdr:colOff>
+      <xdr:colOff>559800</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1624,8 +1639,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8398800" y="10285560"/>
-          <a:ext cx="289440" cy="499680"/>
+          <a:off x="8411400" y="10285560"/>
+          <a:ext cx="289080" cy="499320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1646,9 +1661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>585000</xdr:colOff>
+      <xdr:colOff>584640</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1661,8 +1676,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7456680" y="10604880"/>
-          <a:ext cx="443520" cy="402840"/>
+          <a:off x="7468200" y="10604880"/>
+          <a:ext cx="443160" cy="402480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1683,9 +1698,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>658800</xdr:colOff>
+      <xdr:colOff>658440</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1698,8 +1713,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8331120" y="10900080"/>
-          <a:ext cx="455760" cy="439200"/>
+          <a:off x="8343720" y="10900080"/>
+          <a:ext cx="455400" cy="438840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1720,9 +1735,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>542160</xdr:colOff>
+      <xdr:colOff>541800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1735,8 +1750,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7438680" y="11255040"/>
-          <a:ext cx="418680" cy="426240"/>
+          <a:off x="7450200" y="11255040"/>
+          <a:ext cx="418320" cy="425880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1757,9 +1772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>448920</xdr:colOff>
+      <xdr:colOff>448560</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1772,8 +1787,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8146800" y="11610000"/>
-          <a:ext cx="430200" cy="445680"/>
+          <a:off x="8159400" y="11610000"/>
+          <a:ext cx="429840" cy="445320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1794,9 +1809,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>474120</xdr:colOff>
+      <xdr:colOff>473760</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1809,8 +1824,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7506000" y="11887200"/>
-          <a:ext cx="283320" cy="608040"/>
+          <a:off x="7517520" y="11887200"/>
+          <a:ext cx="282960" cy="607680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1831,9 +1846,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>617040</xdr:colOff>
+      <xdr:colOff>616680</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1846,8 +1861,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8269560" y="4018320"/>
-          <a:ext cx="475560" cy="542160"/>
+          <a:off x="8282160" y="4018320"/>
+          <a:ext cx="475200" cy="541800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1868,9 +1883,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>592560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1883,8 +1898,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7432200" y="4451760"/>
-          <a:ext cx="475560" cy="428040"/>
+          <a:off x="7443720" y="4451760"/>
+          <a:ext cx="475200" cy="427680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1905,9 +1920,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>537120</xdr:colOff>
+      <xdr:colOff>536760</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1920,8 +1935,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8189640" y="12230280"/>
-          <a:ext cx="475560" cy="466200"/>
+          <a:off x="8202240" y="12230280"/>
+          <a:ext cx="475200" cy="465840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1942,9 +1957,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>586440</xdr:colOff>
+      <xdr:colOff>586080</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1957,8 +1972,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7426080" y="12530880"/>
-          <a:ext cx="475560" cy="418680"/>
+          <a:off x="7437600" y="12530880"/>
+          <a:ext cx="475200" cy="418320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1979,9 +1994,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>592560</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>592200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1994,8 +2009,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8245080" y="12772800"/>
-          <a:ext cx="475560" cy="590040"/>
+          <a:off x="8257680" y="12772800"/>
+          <a:ext cx="475200" cy="589680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2016,9 +2031,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>568080</xdr:colOff>
+      <xdr:colOff>567720</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2031,8 +2046,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7407720" y="13187520"/>
-          <a:ext cx="475560" cy="399600"/>
+          <a:off x="7419240" y="13187520"/>
+          <a:ext cx="475200" cy="399240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2053,9 +2068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>506520</xdr:colOff>
+      <xdr:colOff>506160</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2068,8 +2083,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8159040" y="13566960"/>
-          <a:ext cx="475560" cy="313920"/>
+          <a:off x="8171640" y="13566960"/>
+          <a:ext cx="475200" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2090,9 +2105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>604800</xdr:colOff>
+      <xdr:colOff>604440</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2105,8 +2120,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7444440" y="13868640"/>
-          <a:ext cx="475560" cy="475560"/>
+          <a:off x="7455960" y="13868640"/>
+          <a:ext cx="475200" cy="475200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2127,9 +2142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>622800</xdr:colOff>
+      <xdr:colOff>622440</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2142,8 +2157,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8275320" y="14229720"/>
-          <a:ext cx="475560" cy="380520"/>
+          <a:off x="8287920" y="14229720"/>
+          <a:ext cx="475200" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2164,9 +2179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>643680</xdr:colOff>
+      <xdr:colOff>643320</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2179,8 +2194,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7483320" y="14533920"/>
-          <a:ext cx="475560" cy="389880"/>
+          <a:off x="7494840" y="14533920"/>
+          <a:ext cx="475200" cy="389520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2201,9 +2216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>629640</xdr:colOff>
+      <xdr:colOff>629280</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2216,8 +2231,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8282160" y="14798160"/>
-          <a:ext cx="475560" cy="580320"/>
+          <a:off x="8294760" y="14798160"/>
+          <a:ext cx="475200" cy="579960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2238,9 +2253,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>636840</xdr:colOff>
+      <xdr:colOff>636480</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2253,8 +2268,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7476480" y="15143400"/>
-          <a:ext cx="475560" cy="428040"/>
+          <a:off x="7488000" y="15143400"/>
+          <a:ext cx="475200" cy="427680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2275,9 +2290,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>704520</xdr:colOff>
+      <xdr:colOff>704160</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2290,8 +2305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8261640" y="16601760"/>
-          <a:ext cx="570960" cy="389880"/>
+          <a:off x="8274240" y="16601760"/>
+          <a:ext cx="570600" cy="389520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2312,9 +2327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>587520</xdr:colOff>
+      <xdr:colOff>587160</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2327,8 +2342,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7427160" y="16954200"/>
-          <a:ext cx="475560" cy="380520"/>
+          <a:off x="7438680" y="16954200"/>
+          <a:ext cx="475200" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2349,9 +2364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>682920</xdr:colOff>
+      <xdr:colOff>682560</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2364,8 +2379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8240040" y="17218800"/>
-          <a:ext cx="570960" cy="485280"/>
+          <a:off x="8252640" y="17218800"/>
+          <a:ext cx="570600" cy="484920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2386,9 +2401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>648000</xdr:colOff>
+      <xdr:colOff>647640</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2401,8 +2416,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7392240" y="17632440"/>
-          <a:ext cx="570960" cy="370800"/>
+          <a:off x="7403760" y="17632440"/>
+          <a:ext cx="570600" cy="370440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2423,9 +2438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>696960</xdr:colOff>
+      <xdr:colOff>696600</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2438,8 +2453,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8254080" y="17896320"/>
-          <a:ext cx="570960" cy="428040"/>
+          <a:off x="8266680" y="17896320"/>
+          <a:ext cx="570600" cy="427680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2460,9 +2475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>711000</xdr:colOff>
+      <xdr:colOff>710640</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2475,8 +2490,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7455240" y="18282240"/>
-          <a:ext cx="570960" cy="408960"/>
+          <a:off x="7466760" y="18282240"/>
+          <a:ext cx="570600" cy="408600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2497,9 +2512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>641160</xdr:colOff>
+      <xdr:colOff>640800</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2512,8 +2527,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8198280" y="18566280"/>
-          <a:ext cx="570960" cy="399600"/>
+          <a:off x="8210880" y="18566280"/>
+          <a:ext cx="570600" cy="399240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2534,9 +2549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
+      <xdr:colOff>654480</xdr:colOff>
       <xdr:row>113</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2549,8 +2564,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7399080" y="18904680"/>
-          <a:ext cx="570960" cy="313920"/>
+          <a:off x="7410600" y="18904680"/>
+          <a:ext cx="570600" cy="313560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2571,9 +2586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>668880</xdr:colOff>
+      <xdr:colOff>668520</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2586,8 +2601,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8226000" y="19074960"/>
-          <a:ext cx="570960" cy="561240"/>
+          <a:off x="8238600" y="19074960"/>
+          <a:ext cx="570600" cy="560880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2608,9 +2623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675720</xdr:colOff>
       <xdr:row>118</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2623,8 +2638,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7420320" y="19480680"/>
-          <a:ext cx="570960" cy="551880"/>
+          <a:off x="7431840" y="19480680"/>
+          <a:ext cx="570600" cy="551520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2645,9 +2660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>619920</xdr:colOff>
+      <xdr:colOff>619560</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2660,8 +2675,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8177040" y="19840320"/>
-          <a:ext cx="570960" cy="523440"/>
+          <a:off x="8189640" y="19840320"/>
+          <a:ext cx="570600" cy="523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2682,9 +2697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>686880</xdr:colOff>
+      <xdr:colOff>686520</xdr:colOff>
       <xdr:row>123</xdr:row>
-      <xdr:rowOff>106920</xdr:rowOff>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2697,8 +2712,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8148960" y="20578680"/>
-          <a:ext cx="666000" cy="323280"/>
+          <a:off x="8161560" y="20578680"/>
+          <a:ext cx="665640" cy="322920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2719,9 +2734,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>696960</xdr:colOff>
+      <xdr:colOff>696600</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2734,8 +2749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7441200" y="20117520"/>
-          <a:ext cx="570960" cy="532800"/>
+          <a:off x="7452720" y="20117520"/>
+          <a:ext cx="570600" cy="532440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2756,9 +2771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
+      <xdr:colOff>689760</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2771,8 +2786,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7434360" y="20808000"/>
-          <a:ext cx="570960" cy="389880"/>
+          <a:off x="7445880" y="20808000"/>
+          <a:ext cx="570600" cy="389520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2793,9 +2808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
+      <xdr:colOff>689760</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>96120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2808,8 +2823,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8247240" y="21161160"/>
-          <a:ext cx="570960" cy="380520"/>
+          <a:off x="8259840" y="21161160"/>
+          <a:ext cx="570600" cy="380160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2830,9 +2845,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>591840</xdr:colOff>
+      <xdr:colOff>591480</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2845,8 +2860,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7336080" y="21425040"/>
-          <a:ext cx="570960" cy="466200"/>
+          <a:off x="7347600" y="21425040"/>
+          <a:ext cx="570600" cy="465840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>168480</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>87840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>648720</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Image 15" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId57"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8309160" y="21695760"/>
+          <a:ext cx="480240" cy="582480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2866,13 +2918,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N130"/>
+  <dimension ref="A3:N132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D95" activeCellId="0" sqref="D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
@@ -2895,1198 +2947,1218 @@
       <c r="K6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="M10" s="0" t="n">
+      <c r="K10" s="7"/>
+      <c r="M10" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="L12" s="0" t="n">
+      <c r="J12" s="7"/>
+      <c r="L12" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="M14" s="0" t="n">
+      <c r="K14" s="7"/>
+      <c r="M14" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="M16" s="0" t="n">
+      <c r="J16" s="7"/>
+      <c r="M16" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="M18" s="0" t="n">
+      <c r="K18" s="7"/>
+      <c r="M18" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="M21" s="0" t="n">
+      <c r="K21" s="8"/>
+      <c r="M21" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="8"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="M23" s="0" t="n">
+      <c r="J23" s="7"/>
+      <c r="M23" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="M25" s="0" t="n">
+      <c r="K25" s="7"/>
+      <c r="M25" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="L27" s="0" t="n">
+      <c r="J27" s="7"/>
+      <c r="L27" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="8"/>
+      <c r="K28" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="H30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J30" s="6"/>
-      <c r="L30" s="0" t="n">
+      <c r="J30" s="7"/>
+      <c r="L30" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="H32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K32" s="6"/>
-      <c r="M32" s="0" t="n">
+      <c r="K32" s="7"/>
+      <c r="M32" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="H34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="M34" s="0" t="n">
+      <c r="J34" s="7"/>
+      <c r="M34" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="6"/>
-      <c r="L37" s="0" t="n">
+      <c r="J37" s="7"/>
+      <c r="L37" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="H39" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K39" s="6"/>
-      <c r="L39" s="0" t="n">
+      <c r="K39" s="7"/>
+      <c r="L39" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H41" s="0" t="s">
+      <c r="H41" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J41" s="6"/>
-      <c r="M41" s="0" t="n">
+      <c r="J41" s="7"/>
+      <c r="M41" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H43" s="0" t="s">
+      <c r="H43" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="6"/>
-      <c r="M43" s="0" t="n">
+      <c r="K43" s="7"/>
+      <c r="M43" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="H45" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="M45" s="0" t="n">
+      <c r="J45" s="7"/>
+      <c r="M45" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="H47" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K47" s="6"/>
-      <c r="M47" s="0" t="n">
+      <c r="K47" s="7"/>
+      <c r="M47" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H49" s="0" t="s">
+      <c r="H49" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J49" s="6"/>
-      <c r="N49" s="0" t="n">
+      <c r="J49" s="7"/>
+      <c r="N49" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="H51" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K51" s="6"/>
-      <c r="M51" s="0" t="n">
+      <c r="K51" s="7"/>
+      <c r="M51" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H53" s="0" t="s">
+      <c r="H53" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J53" s="6"/>
-      <c r="M53" s="0" t="n">
+      <c r="J53" s="7"/>
+      <c r="M53" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H55" s="0" t="s">
+      <c r="H55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="K55" s="6"/>
-      <c r="M55" s="0" t="n">
+      <c r="K55" s="7"/>
+      <c r="M55" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H57" s="0" t="s">
+      <c r="H57" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J57" s="6"/>
-      <c r="M57" s="0" t="n">
+      <c r="J57" s="7"/>
+      <c r="M57" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H59" s="0" t="s">
+      <c r="H59" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K59" s="6"/>
-      <c r="L59" s="0" t="n">
+      <c r="K59" s="7"/>
+      <c r="L59" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H61" s="0" t="s">
+      <c r="H61" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J61" s="6"/>
-      <c r="L61" s="0" t="n">
+      <c r="J61" s="7"/>
+      <c r="L61" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H63" s="0" t="s">
+      <c r="H63" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K63" s="6"/>
-      <c r="M63" s="0" t="n">
+      <c r="K63" s="7"/>
+      <c r="M63" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H65" s="0" t="s">
+      <c r="H65" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J65" s="6"/>
-      <c r="M65" s="0" t="n">
+      <c r="J65" s="7"/>
+      <c r="M65" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H67" s="0" t="s">
+      <c r="H67" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K67" s="6"/>
-      <c r="M67" s="0" t="n">
+      <c r="K67" s="7"/>
+      <c r="M67" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H69" s="0" t="s">
+      <c r="H69" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J69" s="6"/>
-      <c r="M69" s="0" t="n">
+      <c r="J69" s="7"/>
+      <c r="M69" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H71" s="0" t="s">
+      <c r="H71" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K71" s="6"/>
-      <c r="L71" s="0" t="n">
+      <c r="K71" s="7"/>
+      <c r="L71" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+      <c r="A73" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H73" s="0" t="s">
+      <c r="H73" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J73" s="6"/>
-      <c r="L73" s="0" t="n">
+      <c r="J73" s="7"/>
+      <c r="L73" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+      <c r="A75" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H75" s="0" t="s">
+      <c r="H75" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K75" s="6"/>
-      <c r="L75" s="0" t="n">
+      <c r="K75" s="7"/>
+      <c r="L75" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="8"/>
+      <c r="J76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
+      <c r="A77" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H77" s="0" t="s">
+      <c r="H77" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J77" s="6"/>
-      <c r="L77" s="0" t="n">
+      <c r="J77" s="7"/>
+      <c r="L77" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H79" s="0" t="s">
+      <c r="H79" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K79" s="6"/>
-      <c r="M79" s="0" t="n">
+      <c r="K79" s="7"/>
+      <c r="M79" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H81" s="0" t="s">
+      <c r="H81" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J81" s="6"/>
-      <c r="L81" s="0" t="n">
+      <c r="J81" s="7"/>
+      <c r="L81" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
+      <c r="A83" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H83" s="0" t="s">
+      <c r="H83" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="K83" s="6"/>
-      <c r="L83" s="0" t="n">
+      <c r="K83" s="7"/>
+      <c r="L83" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
+      <c r="A85" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H85" s="0" t="s">
+      <c r="H85" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J85" s="6"/>
-      <c r="L85" s="0" t="n">
+      <c r="J85" s="7"/>
+      <c r="L85" s="4" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
+      <c r="A87" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H87" s="0" t="s">
+      <c r="H87" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K87" s="6"/>
+      <c r="K87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
+      <c r="A89" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H89" s="0" t="s">
+      <c r="H89" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="J89" s="6"/>
+      <c r="J89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
+      <c r="A91" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H91" s="0" t="s">
+      <c r="H91" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="0" t="s">
+      <c r="D92" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
+      <c r="A93" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H93" s="0" t="s">
+      <c r="H93" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
+      <c r="A95" s="4" t="n">
         <v>42</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="L95" s="0" t="n">
+      <c r="L95" s="4" t="n">
         <f aca="false">SUM(L10:L88) - 16*3</f>
         <v>25</v>
       </c>
-      <c r="M95" s="0" t="n">
+      <c r="M95" s="4" t="n">
         <f aca="false">SUM(M10:M88)</f>
         <v>36</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
+      <c r="A99" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="0" t="s">
+      <c r="C99" s="4"/>
+      <c r="D99" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H99" s="9" t="s">
+      <c r="H99" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="J99" s="6"/>
-      <c r="M99" s="0" t="n">
+      <c r="J99" s="7"/>
+      <c r="M99" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="0" t="s">
+      <c r="D100" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
+      <c r="A101" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="9"/>
-      <c r="D101" s="0" t="s">
+      <c r="C101" s="4"/>
+      <c r="D101" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="H101" s="9" t="s">
+      <c r="H101" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="K101" s="6"/>
-      <c r="M101" s="0" t="n">
+      <c r="K101" s="7"/>
+      <c r="M101" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="4" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
+      <c r="A103" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D103" s="0" t="s">
+      <c r="D103" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="H103" s="9" t="s">
+      <c r="H103" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I103" s="9"/>
-      <c r="J103" s="10"/>
-      <c r="L103" s="0" t="n">
+      <c r="I103" s="4"/>
+      <c r="J103" s="9"/>
+      <c r="L103" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="0" t="s">
+      <c r="D104" s="4" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
+      <c r="A105" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D105" s="0" t="s">
+      <c r="D105" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H105" s="0" t="s">
+      <c r="H105" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="K105" s="6"/>
-      <c r="M105" s="0" t="n">
+      <c r="K105" s="7"/>
+      <c r="M105" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="0" t="s">
+      <c r="D106" s="4" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="n">
+      <c r="A107" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D107" s="0" t="s">
+      <c r="D107" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H107" s="0" t="s">
+      <c r="H107" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="J107" s="6"/>
-      <c r="M107" s="0" t="n">
+      <c r="J107" s="7"/>
+      <c r="M107" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="0" t="s">
+      <c r="D108" s="4" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
+      <c r="A109" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D109" s="0" t="s">
+      <c r="D109" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H109" s="0" t="s">
+      <c r="H109" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="K109" s="6"/>
-      <c r="M109" s="0" t="n">
+      <c r="K109" s="7"/>
+      <c r="M109" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="0" t="s">
+      <c r="D110" s="4" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="n">
+      <c r="A111" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D111" s="0" t="s">
+      <c r="D111" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H111" s="0" t="s">
+      <c r="H111" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="J111" s="6"/>
-      <c r="M111" s="0" t="n">
+      <c r="J111" s="7"/>
+      <c r="M111" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="0" t="s">
+      <c r="D112" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="n">
+      <c r="A113" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D113" s="0" t="s">
+      <c r="D113" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="H113" s="0" t="s">
+      <c r="H113" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="K113" s="6"/>
-      <c r="M113" s="0" t="n">
+      <c r="K113" s="7"/>
+      <c r="M113" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="n">
+      <c r="A115" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="B115" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="H115" s="0" t="s">
+      <c r="H115" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="J115" s="6"/>
-      <c r="M115" s="0" t="n">
+      <c r="J115" s="7"/>
+      <c r="M115" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="n">
+      <c r="A117" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D117" s="0" t="s">
+      <c r="D117" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H117" s="0" t="s">
+      <c r="H117" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="K117" s="6"/>
-      <c r="L117" s="0" t="n">
+      <c r="K117" s="7"/>
+      <c r="L117" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="n">
+      <c r="A119" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B119" s="0" t="s">
+      <c r="B119" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D119" s="0" t="s">
+      <c r="D119" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H119" s="0" t="s">
+      <c r="H119" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="J119" s="6"/>
-      <c r="M119" s="0" t="n">
+      <c r="J119" s="7"/>
+      <c r="M119" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="n">
+      <c r="A121" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B121" s="0" t="s">
+      <c r="B121" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="0" t="s">
+      <c r="D121" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H121" s="0" t="s">
+      <c r="H121" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="K121" s="6"/>
-      <c r="M121" s="0" t="n">
+      <c r="K121" s="7"/>
+      <c r="M121" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="n">
+      <c r="A123" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B123" s="0" t="s">
+      <c r="B123" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D123" s="0" t="s">
+      <c r="D123" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H123" s="0" t="s">
+      <c r="H123" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="J123" s="6"/>
-      <c r="M123" s="0" t="n">
+      <c r="J123" s="7"/>
+      <c r="M123" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="n">
+      <c r="A125" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B125" s="0" t="s">
+      <c r="B125" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D125" s="0" t="s">
+      <c r="D125" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="H125" s="0" t="s">
+      <c r="H125" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="K125" s="6"/>
+      <c r="K125" s="7"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="n">
+      <c r="A127" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B127" s="0" t="s">
+      <c r="B127" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D127" s="0" t="s">
+      <c r="D127" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H127" s="0" t="s">
+      <c r="H127" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="J127" s="6"/>
+      <c r="J127" s="7"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="n">
+      <c r="A129" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B129" s="0" t="s">
+      <c r="B129" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D129" s="0" t="s">
+      <c r="D129" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H129" s="0" t="s">
+      <c r="H129" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="K129" s="6"/>
+      <c r="K129" s="7"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D130" s="0" t="s">
+      <c r="D130" s="4" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H131" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="J131" s="7"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D132" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>